<commit_message>
Small Scale Config Changes Miscellaneous test fixes
</commit_message>
<xml_diff>
--- a/Config/Calibrations/calibration_1-5th_LBCB1.xlsx
+++ b/Config/Calibrations/calibration_1-5th_LBCB1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="195" windowWidth="18195" windowHeight="11700" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="17820" windowHeight="11985" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tuning" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="57">
   <si>
     <t>Warning</t>
   </si>
@@ -174,14 +174,32 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>Previous Slopes:</t>
+  </si>
+  <si>
+    <t>R-squared value</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>% Difference</t>
+  </si>
+  <si>
+    <t>New Slope:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000000"/>
+  <numFmts count="4">
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -219,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +253,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,11 +287,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -278,11 +303,19 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="40% - Accent6" xfId="1" builtinId="51"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -726,11 +759,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:T38"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
@@ -774,6 +811,10 @@
       <c r="I7">
         <v>0.875</v>
       </c>
+      <c r="M7">
+        <f>2*0.05</f>
+        <v>0.1</v>
+      </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
@@ -803,34 +844,32 @@
         <f>H8</f>
         <v>6.25</v>
       </c>
+      <c r="M8">
+        <f>1*0.05</f>
+        <v>0.05</v>
+      </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="D9">
-        <f>5+5/16</f>
-        <v>5.3125</v>
-      </c>
-      <c r="E9">
-        <f>5+4/16</f>
-        <v>5.25</v>
-      </c>
-      <c r="F9">
-        <f>4+4/16</f>
-        <v>4.25</v>
-      </c>
-      <c r="G9">
-        <f>4+4/16</f>
-        <v>4.25</v>
-      </c>
-      <c r="H9">
-        <f>4+4/16</f>
-        <v>4.25</v>
-      </c>
-      <c r="I9">
-        <f>4+3/16</f>
-        <v>4.1875</v>
+      <c r="D9" s="9">
+        <v>5.3579999999999997</v>
+      </c>
+      <c r="E9" s="9">
+        <v>5.3860000000000001</v>
+      </c>
+      <c r="F9" s="9">
+        <v>4.3535000000000004</v>
+      </c>
+      <c r="G9" s="9">
+        <v>4.2939999999999996</v>
+      </c>
+      <c r="H9" s="9">
+        <v>4.242</v>
+      </c>
+      <c r="I9" s="9">
+        <v>4.3815</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
@@ -842,27 +881,27 @@
       </c>
       <c r="D10">
         <f>SUM(D7:D9)</f>
-        <v>14.8125</v>
+        <v>14.858000000000001</v>
       </c>
       <c r="E10">
         <f t="shared" ref="E10:I10" si="0">SUM(E7:E9)</f>
-        <v>14.75</v>
+        <v>14.885999999999999</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>11.375</v>
+        <v>11.4785</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>11.375</v>
+        <v>11.419</v>
       </c>
       <c r="H10">
         <f>SUM(H7:H9)</f>
-        <v>11.375</v>
+        <v>11.367000000000001</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>11.3125</v>
+        <v>11.506499999999999</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
@@ -901,27 +940,27 @@
       </c>
       <c r="D12">
         <f>D11-D10</f>
-        <v>-0.36647339958146041</v>
+        <v>-0.41197339958146095</v>
       </c>
       <c r="E12">
         <f t="shared" ref="E12:I12" si="1">E11-E10</f>
-        <v>-0.30397339958146041</v>
+        <v>-0.43997339958145965</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
-        <v>-5.7766972885996637E-2</v>
+        <v>-0.16126697288599701</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>-0.36499102543508322</v>
+        <v>-0.4089910254350837</v>
       </c>
       <c r="H12">
         <f t="shared" si="1"/>
-        <v>-0.36496844237038317</v>
+        <v>-0.35696844237038405</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>-0.30246844237038317</v>
+        <v>-0.49646844237038223</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
@@ -930,27 +969,27 @@
       </c>
       <c r="D13">
         <f>calibration!$F$27</f>
-        <v>0.27375622714345149</v>
+        <v>0.26773623149939174</v>
       </c>
       <c r="E13">
         <f>calibration!$L$27</f>
-        <v>0.27318441842715224</v>
+        <v>0.26755083133801272</v>
       </c>
       <c r="F13">
-        <f>calibration!$F$50</f>
-        <v>0.13428172907023248</v>
+        <f>calibration!$F$53</f>
+        <v>0.13501478873891026</v>
       </c>
       <c r="G13">
-        <f>calibration!$L$50</f>
-        <v>0.13520264780016397</v>
+        <f>calibration!$L$53</f>
+        <v>0.13519771607008962</v>
       </c>
       <c r="H13">
-        <f>calibration!$F$74</f>
-        <v>0.13280936201772017</v>
+        <f>calibration!$F$79</f>
+        <v>0.12608102115425956</v>
       </c>
       <c r="I13">
-        <f>calibration!$L$74</f>
-        <v>0.41117825380426376</v>
+        <f>calibration!$L$79</f>
+        <v>0.40890683932975469</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
@@ -959,56 +998,56 @@
       </c>
       <c r="D14">
         <f>1/D13</f>
-        <v>3.6528849423249401</v>
+        <v>3.7350193300314376</v>
       </c>
       <c r="E14">
         <f t="shared" ref="E14:I14" si="2">1/E13</f>
-        <v>3.6605308815102187</v>
+        <v>3.7376075230229473</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>7.4470295171502947</v>
+        <v>7.4065960428511737</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>7.3963048525354935</v>
+        <v>7.3965746542757929</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>7.5295896675309262</v>
+        <v>7.9314078427117467</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>2.4320352322816112</v>
+        <v>2.445544813188048</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="11">
         <f>D36</f>
-        <v>-0.10305609010989011</v>
-      </c>
-      <c r="E15">
+        <v>-0.10326591758241759</v>
+      </c>
+      <c r="E15" s="11">
         <f>G36</f>
-        <v>-0.10384854835164835</v>
-      </c>
-      <c r="F15">
+        <v>-0.10325958681318681</v>
+      </c>
+      <c r="F15" s="11">
         <f>J36</f>
-        <v>-0.10287610659340658</v>
-      </c>
-      <c r="G15">
+        <v>-0.10287267802197804</v>
+      </c>
+      <c r="G15" s="11">
         <f>M36</f>
-        <v>-0.10246634065934067</v>
-      </c>
-      <c r="H15">
+        <v>-0.10240945494505495</v>
+      </c>
+      <c r="H15" s="11">
         <f>P36</f>
-        <v>-0.10322215934065933</v>
-      </c>
-      <c r="I15">
+        <v>-0.10259925054945054</v>
+      </c>
+      <c r="I15" s="11">
         <f>S36</f>
-        <v>-0.10256173999999998</v>
+        <v>-0.10253797191780821</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
@@ -1017,80 +1056,80 @@
       </c>
       <c r="D16">
         <f>1/D15</f>
-        <v>-9.7034537108256913</v>
+        <v>-9.6837371265489391</v>
       </c>
       <c r="E16">
         <f t="shared" ref="E16:I16" si="3">1/E15</f>
-        <v>-9.6294075928132834</v>
+        <v>-9.6843308293414037</v>
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>-9.7204300698534691</v>
+        <v>-9.7207540352585831</v>
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
-        <v>-9.7593023578796227</v>
+        <v>-9.7647233894226204</v>
       </c>
       <c r="H16">
         <f t="shared" si="3"/>
-        <v>-9.6878422849084771</v>
+        <v>-9.7466598892749445</v>
       </c>
       <c r="I16">
         <f t="shared" si="3"/>
-        <v>-9.7502245964235801</v>
+        <v>-9.7524846775941132</v>
       </c>
       <c r="K16">
         <f>D14*D16</f>
-        <v>-35.445599948822235</v>
+        <v>-36.16894535460338</v>
       </c>
       <c r="L16">
         <f t="shared" ref="L16:P16" si="4">E14*E16</f>
-        <v>-35.248743864142</v>
+        <v>-36.196227763189491</v>
       </c>
       <c r="M16">
         <f t="shared" si="4"/>
-        <v>-72.388329649594084</v>
+        <v>-71.997698371075799</v>
       </c>
       <c r="N16">
         <f t="shared" si="4"/>
-        <v>-72.182775386946133</v>
+        <v>-72.225505528217369</v>
       </c>
       <c r="O16">
         <f t="shared" si="4"/>
-        <v>-72.945477169116074</v>
+        <v>-77.304734686039296</v>
       </c>
       <c r="P16">
         <f t="shared" si="4"/>
-        <v>-23.7128897411609</v>
+        <v>-23.850138318986197</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="13">
         <f>D12*D14*D16</f>
-        <v>12.989869513449323</v>
-      </c>
-      <c r="E17">
+        <v>14.900643377012043</v>
+      </c>
+      <c r="E17" s="13">
         <f t="shared" ref="E17:I17" si="5">E12*E14*E16</f>
-        <v>10.714680503359387</v>
-      </c>
-      <c r="F17">
+        <v>15.925377380995291</v>
+      </c>
+      <c r="F17" s="13">
         <f t="shared" si="5"/>
-        <v>4.1816546761306883</v>
-      </c>
-      <c r="G17">
+        <v>11.610850871062473</v>
+      </c>
+      <c r="G17" s="13">
         <f t="shared" si="5"/>
-        <v>26.346065207231756</v>
-      </c>
-      <c r="H17">
+        <v>29.539583568552928</v>
+      </c>
+      <c r="H17" s="13">
         <f t="shared" si="5"/>
-        <v>26.622797180376637</v>
-      </c>
-      <c r="I17">
+        <v>27.595350728731248</v>
+      </c>
+      <c r="I17" s="13">
         <f t="shared" si="5"/>
-        <v>7.1724008241095758</v>
+        <v>11.840841021545243</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -1154,22 +1193,40 @@
         <v>17</v>
       </c>
       <c r="D20">
-        <v>75.05</v>
+        <v>73.67</v>
       </c>
       <c r="E20">
-        <v>-7.7741400000000001</v>
+        <v>-7.5970199999999997</v>
       </c>
       <c r="G20">
-        <v>72.364999999999995</v>
+        <v>75.349999999999994</v>
       </c>
       <c r="H20">
-        <v>-7.4498800000000003</v>
+        <v>-7.7512299999999996</v>
       </c>
       <c r="J20">
-        <v>74.088999999999999</v>
+        <v>74.319999999999993</v>
       </c>
       <c r="K20">
-        <v>-7.6451200000000004</v>
+        <v>-7.6415899999999999</v>
+      </c>
+      <c r="M20">
+        <v>70.48</v>
+      </c>
+      <c r="N20">
+        <v>-7.2399100000000001</v>
+      </c>
+      <c r="P20">
+        <v>73.5</v>
+      </c>
+      <c r="Q20">
+        <v>-7.5611800000000002</v>
+      </c>
+      <c r="S20">
+        <v>21.73</v>
+      </c>
+      <c r="T20">
+        <v>-2.2019099999999998</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -1177,474 +1234,496 @@
         <v>18</v>
       </c>
       <c r="D21">
-        <v>-70.463999999999999</v>
+        <v>-71.25</v>
       </c>
       <c r="E21">
-        <v>7.2832100000000004</v>
+        <v>7.4077500000000001</v>
       </c>
       <c r="G21">
-        <v>-72.284999999999997</v>
+        <v>-70.510000000000005</v>
       </c>
       <c r="H21">
-        <v>7.4453100000000001</v>
+        <v>7.3595199999999998</v>
       </c>
       <c r="J21">
-        <v>-72.435000000000002</v>
+        <v>-70.739999999999995</v>
       </c>
       <c r="K21">
-        <v>7.4670699999999997</v>
+        <v>7.3195600000000001</v>
+      </c>
+      <c r="M21">
+        <v>-72.650000000000006</v>
+      </c>
+      <c r="N21">
+        <v>7.46265</v>
+      </c>
+      <c r="P21">
+        <v>-77.739999999999995</v>
+      </c>
+      <c r="Q21">
+        <v>7.9522500000000003</v>
+      </c>
+      <c r="S21">
+        <v>-18.38</v>
+      </c>
+      <c r="T21">
+        <v>1.90343</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="12">
         <f>(D20+D21)*0.5</f>
-        <v>2.2929999999999993</v>
-      </c>
+        <v>1.2100000000000009</v>
+      </c>
+      <c r="E22" s="11"/>
       <c r="G22" s="4">
         <f>(G20+G21)*0.5</f>
-        <v>3.9999999999999147E-2</v>
+        <v>2.4199999999999946</v>
       </c>
       <c r="J22" s="4">
         <f>(J20+J21)*0.5</f>
-        <v>0.82699999999999818</v>
-      </c>
-      <c r="M22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="S22" s="4"/>
+        <v>1.7899999999999991</v>
+      </c>
+      <c r="M22" s="4">
+        <f>(M20+M21)*0.5</f>
+        <v>-1.0850000000000009</v>
+      </c>
+      <c r="P22" s="4">
+        <f>(P20+P21)*0.5</f>
+        <v>-2.1199999999999974</v>
+      </c>
+      <c r="S22" s="4">
+        <f>(S20+S21)*0.5</f>
+        <v>1.6750000000000007</v>
+      </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D23">
+      <c r="D23" s="11">
         <v>5</v>
       </c>
-      <c r="E23">
-        <v>-0.51108799999999999</v>
+      <c r="E23" s="11">
+        <v>-0.48705100000000001</v>
       </c>
       <c r="G23">
         <v>5</v>
       </c>
       <c r="H23">
-        <v>-0.53189799999999998</v>
+        <v>-0.45359100000000002</v>
       </c>
       <c r="J23">
         <v>5</v>
       </c>
       <c r="K23">
-        <v>-0.51057699999999995</v>
+        <v>-0.49504300000000001</v>
       </c>
       <c r="M23">
         <v>5</v>
       </c>
       <c r="N23">
-        <v>-0.508243</v>
+        <v>-0.51510500000000004</v>
       </c>
       <c r="P23">
         <v>5</v>
       </c>
       <c r="Q23">
-        <v>-0.48058800000000002</v>
+        <v>-0.56676599999999999</v>
       </c>
       <c r="S23">
         <v>5</v>
       </c>
       <c r="T23">
-        <v>-0.53745200000000004</v>
+        <v>-0.49207400000000001</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D24">
+      <c r="D24" s="11">
         <v>10</v>
       </c>
-      <c r="E24">
-        <v>-1.0248999999999999</v>
+      <c r="E24" s="11">
+        <v>-1.0029600000000001</v>
       </c>
       <c r="G24">
         <v>10</v>
       </c>
       <c r="H24">
-        <v>-1.05698</v>
+        <v>-0.97196800000000005</v>
       </c>
       <c r="J24">
         <v>10</v>
       </c>
       <c r="K24">
-        <v>-1.02136</v>
+        <v>-1.00945</v>
       </c>
       <c r="M24">
         <v>10</v>
       </c>
       <c r="N24">
-        <v>-1.02173</v>
+        <v>-1.0283800000000001</v>
       </c>
       <c r="P24">
         <v>10</v>
       </c>
       <c r="Q24">
-        <v>-0.996166</v>
+        <v>-1.07663</v>
       </c>
       <c r="S24">
         <v>10</v>
       </c>
       <c r="T24">
-        <v>-1.0499799999999999</v>
+        <v>-1.0032700000000001</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D25">
+      <c r="D25" s="11">
         <v>15</v>
       </c>
-      <c r="E25">
-        <v>-1.5410200000000001</v>
+      <c r="E25" s="11">
+        <v>-1.51851</v>
       </c>
       <c r="G25">
         <v>15</v>
       </c>
       <c r="H25">
-        <v>-1.57524</v>
+        <v>-1.4873400000000001</v>
       </c>
       <c r="J25">
         <v>15</v>
       </c>
       <c r="K25">
-        <v>-1.54877</v>
+        <v>-1.52285</v>
       </c>
       <c r="M25">
         <v>15</v>
       </c>
       <c r="N25">
-        <v>-1.53487</v>
+        <v>-1.5386200000000001</v>
       </c>
       <c r="P25">
         <v>15</v>
       </c>
       <c r="Q25">
-        <v>-1.5107900000000001</v>
+        <v>-1.5874299999999999</v>
       </c>
       <c r="S25">
         <v>15</v>
       </c>
       <c r="T25">
-        <v>-1.56426</v>
+        <v>-1.5134300000000001</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D26">
+      <c r="D26" s="11">
         <v>20</v>
       </c>
-      <c r="E26">
-        <v>-2.0536099999999999</v>
+      <c r="E26" s="11">
+        <v>-2.0347</v>
       </c>
       <c r="G26">
         <v>20</v>
       </c>
       <c r="H26">
-        <v>-2.0954100000000002</v>
+        <v>-2.00495</v>
       </c>
       <c r="J26">
         <v>20</v>
       </c>
       <c r="K26">
-        <v>-2.05233</v>
+        <v>-2.0376300000000001</v>
       </c>
       <c r="M26">
         <v>20</v>
       </c>
       <c r="N26">
-        <v>-2.04392</v>
+        <v>-2.0523199999999999</v>
       </c>
       <c r="P26">
         <v>20</v>
       </c>
       <c r="Q26">
-        <v>-2.0276700000000001</v>
+        <v>-2.1009899999999999</v>
       </c>
       <c r="S26">
         <v>20</v>
       </c>
       <c r="T26">
-        <v>-2.0751300000000001</v>
+        <v>-2.02536</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D27">
+      <c r="D27" s="11">
         <v>25</v>
       </c>
-      <c r="E27">
-        <v>-2.5710700000000002</v>
+      <c r="E27" s="11">
+        <v>-2.5505</v>
       </c>
       <c r="G27">
         <v>25</v>
       </c>
       <c r="H27">
-        <v>-2.6139299999999999</v>
+        <v>-2.5223300000000002</v>
       </c>
       <c r="J27">
         <v>25</v>
       </c>
       <c r="K27">
-        <v>-2.56427</v>
+        <v>-2.5516399999999999</v>
       </c>
       <c r="M27">
         <v>25</v>
       </c>
       <c r="N27">
-        <v>-2.5581100000000001</v>
+        <v>-2.5645199999999999</v>
       </c>
       <c r="P27">
         <v>25</v>
       </c>
       <c r="Q27">
-        <v>-2.54183</v>
+        <v>-2.6142400000000001</v>
       </c>
       <c r="S27">
         <v>-5</v>
       </c>
       <c r="T27">
-        <v>0.48718</v>
+        <v>0.53804700000000005</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D28">
+      <c r="D28" s="11">
         <v>30</v>
       </c>
-      <c r="E28">
-        <v>-3.0871</v>
+      <c r="E28" s="11">
+        <v>-3.0677400000000001</v>
       </c>
       <c r="G28">
         <v>30</v>
       </c>
       <c r="H28">
-        <v>-3.1337299999999999</v>
+        <v>-3.0382199999999999</v>
       </c>
       <c r="J28">
         <v>30</v>
       </c>
       <c r="K28">
-        <v>-3.0803400000000001</v>
+        <v>-3.0653299999999999</v>
       </c>
       <c r="M28">
         <v>30</v>
       </c>
       <c r="N28">
-        <v>-3.0707900000000001</v>
+        <v>-3.0770599999999999</v>
       </c>
       <c r="P28">
         <v>30</v>
       </c>
       <c r="Q28">
-        <v>-3.05741</v>
+        <v>-3.12466</v>
       </c>
       <c r="S28">
         <v>-10</v>
       </c>
       <c r="T28">
-        <v>1.0017400000000001</v>
+        <v>1.0498499999999999</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D29">
+      <c r="D29" s="11">
         <v>-5</v>
       </c>
-      <c r="E29">
-        <v>0.52249400000000001</v>
+      <c r="E29" s="11">
+        <v>0.54721399999999998</v>
       </c>
       <c r="G29">
         <v>-5</v>
       </c>
       <c r="H29">
-        <v>0.50017100000000003</v>
+        <v>0.57637700000000003</v>
       </c>
       <c r="J29">
         <v>-5</v>
       </c>
       <c r="K29">
-        <v>0.52061000000000002</v>
+        <v>0.53343399999999996</v>
       </c>
       <c r="M29">
         <v>-5</v>
       </c>
       <c r="N29">
-        <v>0.516517</v>
+        <v>0.50778900000000005</v>
       </c>
       <c r="P29">
         <v>-5</v>
       </c>
       <c r="Q29">
-        <v>0.55500499999999997</v>
+        <v>0.46515800000000002</v>
       </c>
       <c r="S29">
         <v>-15</v>
       </c>
       <c r="T29">
-        <v>1.51261</v>
+        <v>1.56175</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D30">
+      <c r="D30" s="11">
         <v>-10</v>
       </c>
-      <c r="E30">
-        <v>1.03363</v>
+      <c r="E30" s="11">
+        <v>1.0638700000000001</v>
       </c>
       <c r="G30">
         <v>-10</v>
       </c>
       <c r="H30">
-        <v>1.0186299999999999</v>
+        <v>1.09192</v>
       </c>
       <c r="J30">
         <v>-10</v>
       </c>
       <c r="K30">
-        <v>1.03447</v>
+        <v>1.04637</v>
       </c>
       <c r="M30">
         <v>-10</v>
       </c>
       <c r="N30">
-        <v>1.0254799999999999</v>
+        <v>1.0203100000000001</v>
       </c>
       <c r="P30">
         <v>-10</v>
       </c>
       <c r="Q30">
-        <v>1.0701099999999999</v>
-      </c>
-      <c r="S30">
-        <v>-20</v>
-      </c>
-      <c r="T30">
-        <v>2.0273300000000001</v>
+        <v>0.978132</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D31">
+      <c r="D31" s="11">
         <v>-15</v>
       </c>
-      <c r="E31">
-        <v>1.5500100000000001</v>
+      <c r="E31" s="11">
+        <v>1.57911</v>
       </c>
       <c r="G31">
         <v>-15</v>
       </c>
       <c r="H31">
-        <v>1.54278</v>
+        <v>1.6089800000000001</v>
       </c>
       <c r="J31">
         <v>-15</v>
       </c>
       <c r="K31">
-        <v>1.54617</v>
+        <v>1.56219</v>
       </c>
       <c r="M31">
         <v>-15</v>
       </c>
       <c r="N31">
-        <v>1.5388500000000001</v>
+        <v>1.53121</v>
       </c>
       <c r="P31">
         <v>-15</v>
       </c>
       <c r="Q31">
-        <v>1.5835699999999999</v>
+        <v>1.4900199999999999</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D32">
+      <c r="D32" s="11">
         <v>-20</v>
       </c>
-      <c r="E32">
-        <v>2.06792</v>
+      <c r="E32" s="11">
+        <v>2.0959500000000002</v>
       </c>
       <c r="G32">
         <v>-20</v>
       </c>
       <c r="H32">
-        <v>2.0629599999999999</v>
+        <v>2.1241500000000002</v>
       </c>
       <c r="J32">
         <v>-20</v>
       </c>
       <c r="K32">
-        <v>2.06243</v>
+        <v>2.0761699999999998</v>
       </c>
       <c r="M32">
         <v>-20</v>
       </c>
       <c r="N32">
-        <v>2.05349</v>
+        <v>2.0444300000000002</v>
       </c>
       <c r="P32">
         <v>-20</v>
       </c>
       <c r="Q32">
-        <v>2.1023499999999999</v>
+        <v>2.00345</v>
       </c>
     </row>
     <row r="33" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="D33">
+      <c r="D33" s="11">
         <v>-25</v>
       </c>
-      <c r="E33">
-        <v>2.58196</v>
+      <c r="E33" s="11">
+        <v>2.6114199999999999</v>
       </c>
       <c r="G33">
         <v>-25</v>
       </c>
       <c r="H33">
-        <v>2.5767000000000002</v>
+        <v>2.6427100000000001</v>
       </c>
       <c r="J33">
         <v>-25</v>
       </c>
       <c r="K33">
-        <v>2.5776599999999998</v>
+        <v>2.59362</v>
       </c>
       <c r="M33">
         <v>-25</v>
       </c>
       <c r="N33">
-        <v>2.56562</v>
+        <v>2.5558200000000002</v>
       </c>
       <c r="P33">
         <v>-25</v>
       </c>
       <c r="Q33">
-        <v>2.6185499999999999</v>
+        <v>2.51702</v>
       </c>
     </row>
     <row r="34" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="D34">
+      <c r="D34" s="11">
         <v>-30</v>
       </c>
-      <c r="E34">
-        <v>3.0972400000000002</v>
+      <c r="E34" s="11">
+        <v>3.1287600000000002</v>
       </c>
       <c r="G34">
         <v>-30</v>
       </c>
       <c r="H34">
-        <v>3.0959699999999999</v>
+        <v>3.1581000000000001</v>
       </c>
       <c r="J34">
         <v>-30</v>
       </c>
       <c r="K34">
-        <v>3.0898099999999999</v>
+        <v>3.1075699999999999</v>
       </c>
       <c r="M34">
         <v>-30</v>
       </c>
       <c r="N34">
-        <v>3.0785</v>
+        <v>3.0686300000000002</v>
       </c>
       <c r="P34">
         <v>-30</v>
       </c>
       <c r="Q34">
-        <v>3.1357499999999998</v>
+        <v>3.0282499999999999</v>
       </c>
     </row>
     <row r="35" spans="3:20" x14ac:dyDescent="0.25">
@@ -1652,11 +1731,11 @@
         <f>"y="</f>
         <v>y=</v>
       </c>
-      <c r="D35" t="str">
+      <c r="D35" s="11" t="str">
         <f>"Ax"</f>
         <v>Ax</v>
       </c>
-      <c r="E35" t="str">
+      <c r="E35" s="11" t="str">
         <f>"+B"</f>
         <v>+B</v>
       </c>
@@ -1722,54 +1801,60 @@
       </c>
     </row>
     <row r="36" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="D36">
+      <c r="D36" s="11">
         <f>SLOPE(E23:E34,D23:D34)</f>
-        <v>-0.10305609010989011</v>
-      </c>
-      <c r="E36">
+        <v>-0.10326591758241759</v>
+      </c>
+      <c r="E36" s="11">
         <f>1/12*(SUM(E23:E34)-SUM(D23:D34)*D36)</f>
-        <v>5.3721666666667334E-3</v>
+        <v>3.0405249999999939E-2</v>
       </c>
       <c r="G36">
         <f>SLOPE(H23:H34,G23:G34)</f>
-        <v>-0.10384854835164835</v>
+        <v>-0.10325958681318681</v>
       </c>
       <c r="H36">
         <f>1/12*(SUM(H23:H34)-SUM(G23:G34)*G36)</f>
-        <v>-1.7498083333333209E-2</v>
+        <v>6.0319833333333461E-2</v>
       </c>
       <c r="J36">
         <f>SLOPE(K23:K34,J23:J34)</f>
-        <v>-0.10287610659340658</v>
+        <v>-0.10287267802197804</v>
       </c>
       <c r="K36">
         <f>1/12*(SUM(K23:K34)-SUM(J23:J34)*J36)</f>
-        <v>4.4585833333333396E-3</v>
+        <v>1.9784249999999948E-2</v>
       </c>
       <c r="M36">
         <f>SLOPE(N23:N34,M23:M34)</f>
-        <v>-0.10246634065934067</v>
+        <v>-0.10240945494505495</v>
       </c>
       <c r="N36">
         <f>1/12*(SUM(N23:N34)-SUM(M23:M34)*M36)</f>
-        <v>3.3995000000000735E-3</v>
+        <v>-3.9846666666665254E-3</v>
       </c>
       <c r="P36">
         <f>SLOPE(Q23:Q34,P23:P34)</f>
-        <v>-0.10322215934065933</v>
+        <v>-0.10259925054945054</v>
       </c>
       <c r="Q36">
         <f>1/12*(SUM(Q23:Q34)-SUM(P23:P34)*P36)</f>
-        <v>3.7573416666666505E-2</v>
+        <v>-4.9057166666666707E-2</v>
       </c>
       <c r="S36">
         <f>SLOPE(T23:T32,S23:S32)</f>
-        <v>-0.10256173999999998</v>
+        <v>-0.10253797191780821</v>
       </c>
       <c r="T36">
         <f>1/12*(SUM(T23:T32)-SUM(S23:S32)*S36)</f>
-        <v>-1.6496833333333329E-2</v>
-      </c>
+        <v>1.3856036529680333E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="J37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="S37" s="10"/>
     </row>
     <row r="38" spans="3:20" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
@@ -1799,7 +1884,7 @@
   <dimension ref="A3:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:L75"/>
+  <dimension ref="C6:L84"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="L69" sqref="L69"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,19 +2148,19 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>3.3975899999999998E-3</v>
+        <v>-1.31745</v>
       </c>
       <c r="F9">
-        <v>2.1349999999999998</v>
+        <v>1.8160000000000001</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>-1.3950000000000001E-2</v>
+        <v>-1.0486899999999999</v>
       </c>
       <c r="L9">
-        <v>2.1110000000000002</v>
+        <v>1.8759999999999999</v>
       </c>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.25">
@@ -2083,19 +2168,19 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>-0.98993600000000004</v>
+        <v>-2.3213300000000001</v>
       </c>
       <c r="F10">
-        <v>1.893</v>
+        <v>1.546</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>-1.0178400000000001</v>
+        <v>-2.0520700000000001</v>
       </c>
       <c r="L10">
-        <v>1.8360000000000001</v>
+        <v>1.605</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.25">
@@ -2103,19 +2188,19 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <v>-1.9837100000000001</v>
+        <v>-3.3243499999999999</v>
       </c>
       <c r="F11">
-        <v>1.589</v>
+        <v>1.2789999999999999</v>
       </c>
       <c r="J11">
         <v>2</v>
       </c>
       <c r="K11">
-        <v>-2.02251</v>
+        <v>-3.0554299999999999</v>
       </c>
       <c r="L11">
-        <v>1.5669999999999999</v>
+        <v>1.341</v>
       </c>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
@@ -2123,139 +2208,139 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>-2.97715</v>
+        <v>-4.3279899999999998</v>
       </c>
       <c r="F12">
-        <v>1.325</v>
+        <v>1.006</v>
       </c>
       <c r="J12">
         <v>3</v>
       </c>
       <c r="K12">
-        <v>-3.0278200000000002</v>
+        <v>-4.0589399999999998</v>
       </c>
       <c r="L12">
-        <v>1.2909999999999999</v>
+        <v>1.073</v>
       </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>-3.9693700000000001</v>
+        <v>-3.3225799999999999</v>
       </c>
       <c r="F13">
-        <v>1.0509999999999999</v>
+        <v>1.2789999999999999</v>
       </c>
       <c r="J13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K13">
-        <v>-4.0327500000000001</v>
+        <v>-3.0541999999999998</v>
       </c>
       <c r="L13">
-        <v>1.0209999999999999</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>-2.9754499999999999</v>
+        <v>-2.31785</v>
       </c>
       <c r="F14">
-        <v>1.329</v>
+        <v>1.552</v>
       </c>
       <c r="J14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K14">
-        <v>-3.0275500000000002</v>
+        <v>-2.0508199999999999</v>
       </c>
       <c r="L14">
-        <v>1.2929999999999999</v>
+        <v>1.607</v>
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>-1.98244</v>
+        <v>-1.3135399999999999</v>
       </c>
       <c r="F15">
-        <v>1.603</v>
+        <v>1.821</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>-2.0227300000000001</v>
+        <v>-1.0479499999999999</v>
       </c>
       <c r="L15">
-        <v>1.5640000000000001</v>
+        <v>1.873</v>
       </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E16">
-        <v>-0.98838999999999999</v>
+        <v>-0.30986599999999997</v>
       </c>
       <c r="F16">
-        <v>1.86</v>
+        <v>2.0910000000000002</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="K16">
-        <v>-1.0179199999999999</v>
+        <v>-4.5754599999999999E-2</v>
       </c>
       <c r="L16">
-        <v>1.8380000000000001</v>
+        <v>2.1419999999999999</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D17">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E17">
-        <v>5.3801600000000002E-3</v>
+        <v>0.69376700000000002</v>
       </c>
       <c r="F17">
-        <v>2.141</v>
+        <v>2.351</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K17">
-        <v>-1.3027800000000001E-2</v>
+        <v>0.95646600000000004</v>
       </c>
       <c r="L17">
-        <v>2.1120000000000001</v>
+        <v>2.4129999999999998</v>
       </c>
     </row>
     <row r="18" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D18">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="E18">
-        <v>0.99950799999999995</v>
+        <v>1.6964699999999999</v>
       </c>
       <c r="F18">
-        <v>2.4119999999999999</v>
+        <v>2.6190000000000002</v>
       </c>
       <c r="J18">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="K18">
-        <v>0.992232</v>
+        <v>1.95733</v>
       </c>
       <c r="L18">
-        <v>2.3860000000000001</v>
+        <v>2.6760000000000002</v>
       </c>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.25">
@@ -2263,157 +2348,105 @@
         <v>-2</v>
       </c>
       <c r="E19">
-        <v>1.99352</v>
+        <v>0.69452999999999998</v>
       </c>
       <c r="F19">
-        <v>2.694</v>
+        <v>2.3540000000000001</v>
       </c>
       <c r="J19">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="K19">
-        <v>1.99715</v>
+        <v>2.9580099999999998</v>
       </c>
       <c r="L19">
-        <v>2.6619999999999999</v>
+        <v>2.9489999999999998</v>
       </c>
     </row>
     <row r="20" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D20">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="E20">
-        <v>2.9871300000000001</v>
+        <v>-0.30854900000000002</v>
       </c>
       <c r="F20">
-        <v>2.9550000000000001</v>
+        <v>2.0920000000000001</v>
       </c>
       <c r="J20">
         <v>-3</v>
       </c>
       <c r="K20">
-        <v>3.0016500000000002</v>
+        <v>1.9572499999999999</v>
       </c>
       <c r="L20">
-        <v>2.9390000000000001</v>
+        <v>2.6869999999999998</v>
       </c>
     </row>
     <row r="21" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D21">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>3.9819599999999999</v>
+        <v>-1.3117799999999999</v>
       </c>
       <c r="F21">
-        <v>3.23</v>
+        <v>1.8220000000000001</v>
       </c>
       <c r="J21">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="K21">
-        <v>4.0070800000000002</v>
+        <v>0.95610899999999999</v>
       </c>
       <c r="L21">
-        <v>3.222</v>
+        <v>2.41</v>
       </c>
     </row>
     <row r="22" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D22">
-        <v>-3</v>
-      </c>
-      <c r="E22">
-        <v>2.9876800000000001</v>
-      </c>
-      <c r="F22">
-        <v>2.96</v>
-      </c>
       <c r="J22">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="K22">
-        <v>3.0032299999999998</v>
+        <v>-4.5898500000000002E-2</v>
       </c>
       <c r="L22">
-        <v>2.9390000000000001</v>
+        <v>2.1440000000000001</v>
       </c>
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D23">
-        <v>-2</v>
-      </c>
-      <c r="E23">
-        <v>1.9939</v>
-      </c>
-      <c r="F23">
-        <v>2.6880000000000002</v>
-      </c>
       <c r="J23">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="K23">
-        <v>1.99807</v>
+        <v>-1.0487200000000001</v>
       </c>
       <c r="L23">
-        <v>2.657</v>
-      </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D24">
-        <v>-1</v>
-      </c>
-      <c r="E24">
-        <v>0.99942299999999995</v>
-      </c>
-      <c r="F24">
-        <v>2.4079999999999999</v>
-      </c>
-      <c r="J24">
-        <v>-1</v>
-      </c>
-      <c r="K24">
-        <v>0.99310699999999996</v>
-      </c>
-      <c r="L24">
-        <v>2.387</v>
-      </c>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>6.0303500000000003E-3</v>
-      </c>
-      <c r="F25">
-        <v>2.1389999999999998</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>-1.19296E-2</v>
-      </c>
-      <c r="L25">
-        <v>2.1190000000000002</v>
+        <v>1.871</v>
       </c>
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
       <c r="E27">
         <f>SLOPE(F9:F25,D9:D25)</f>
-        <v>-0.27211363636363639</v>
+        <v>-0.26889473684210524</v>
       </c>
       <c r="F27">
         <f>SLOPE(F9:F25,E9:E25)</f>
-        <v>0.27375622714345149</v>
+        <v>0.26773623149939174</v>
+      </c>
+      <c r="I27" t="s">
+        <v>56</v>
       </c>
       <c r="K27">
         <f>SLOPE(L9:L25,J9:J25)</f>
-        <v>-0.27455681818181821</v>
+        <v>-0.26820424107142854</v>
       </c>
       <c r="L27">
         <f>SLOPE(L9:L25,K9:K25)</f>
-        <v>0.27318441842715224</v>
+        <v>0.26755083133801272</v>
       </c>
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.25">
@@ -2430,662 +2463,932 @@
         <v>33</v>
       </c>
     </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29">
+        <f>RSQ(E9:E25,D9:D25)</f>
+        <v>0.99999913869274848</v>
+      </c>
+      <c r="F29">
+        <f>RSQ(F9:F25,D9:D25)</f>
+        <v>0.99993565275145813</v>
+      </c>
+      <c r="I29" t="s">
+        <v>53</v>
+      </c>
+      <c r="K29">
+        <f>RSQ(K9:K25,J9:J25)</f>
+        <v>0.99999965578312244</v>
+      </c>
+      <c r="L29">
+        <f>RSQ(L9:L25,J9:J25)</f>
+        <v>0.99997367703219009</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30">
+        <v>-0.27211363636363639</v>
+      </c>
+      <c r="F30">
+        <v>0.27375622714345149</v>
+      </c>
+      <c r="I30" t="s">
+        <v>52</v>
+      </c>
+      <c r="K30">
+        <v>-0.27455681818181821</v>
+      </c>
+      <c r="L30">
+        <v>0.27318441842715224</v>
+      </c>
+    </row>
     <row r="31" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31">
+        <f>E27-E30</f>
+        <v>3.2188995215311489E-3</v>
+      </c>
+      <c r="F31">
+        <f>F27-F30</f>
+        <v>-6.0199956440597502E-3</v>
+      </c>
+      <c r="I31" t="s">
+        <v>54</v>
+      </c>
+      <c r="K31">
+        <f>K27-K30</f>
+        <v>6.3525771103896678E-3</v>
+      </c>
+      <c r="L31">
+        <f>L27-L30</f>
+        <v>-5.6335870891395246E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="8">
+        <f>(E30-E27)/((E27+E30)/2)</f>
+        <v>1.1899629214452194E-2</v>
+      </c>
+      <c r="F32" s="8">
+        <f>(F30-F27)/((F27+F30)/2)</f>
+        <v>2.223482727404117E-2</v>
+      </c>
+      <c r="I32" t="s">
+        <v>55</v>
+      </c>
+      <c r="K32" s="8">
+        <f>(K30-K27)/((K27+K30)/2)</f>
+        <v>2.340837465064206E-2</v>
+      </c>
+      <c r="L32" s="8">
+        <f>(L30-L27)/((L27+L30)/2)</f>
+        <v>2.0836766575088737E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>28</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D34" t="s">
         <v>31</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E34" t="s">
         <v>29</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F34" t="s">
         <v>30</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I34" t="s">
         <v>34</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J34" t="s">
         <v>31</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K34" t="s">
         <v>29</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L34" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D34">
+    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D37">
         <v>0</v>
       </c>
-      <c r="E34">
-        <v>1.64489E-3</v>
-      </c>
-      <c r="F34">
-        <v>1.18</v>
-      </c>
-      <c r="J34">
+      <c r="E37">
+        <v>-0.41559000000000001</v>
+      </c>
+      <c r="F37">
+        <v>1.016</v>
+      </c>
+      <c r="J37">
         <v>0</v>
       </c>
-      <c r="K34">
-        <v>-1.8941699999999999E-3</v>
-      </c>
-      <c r="L34">
-        <v>1.093</v>
-      </c>
-    </row>
-    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D35">
+      <c r="K37">
+        <v>-2.70296</v>
+      </c>
+      <c r="L37">
+        <v>0.69899999999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D38">
         <v>1</v>
       </c>
-      <c r="E35">
-        <v>-0.98804400000000003</v>
-      </c>
-      <c r="F35">
-        <v>1.044</v>
-      </c>
-      <c r="J35">
+      <c r="E38">
+        <v>-1.4087000000000001</v>
+      </c>
+      <c r="F38">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="J38">
+        <v>0.5</v>
+      </c>
+      <c r="K38">
+        <v>-3.1982599999999999</v>
+      </c>
+      <c r="L38">
+        <v>0.627</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>-2.4026200000000002</v>
+      </c>
+      <c r="F39">
+        <v>0.751</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>-2.7044299999999999</v>
+      </c>
+      <c r="L39">
+        <v>0.70099999999999996</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D40">
         <v>1</v>
       </c>
-      <c r="K35">
-        <v>-0.99555199999999999</v>
-      </c>
-      <c r="L35">
-        <v>0.95899999999999996</v>
-      </c>
-    </row>
-    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D36">
-        <v>2</v>
-      </c>
-      <c r="E36">
-        <v>-1.9823200000000001</v>
-      </c>
-      <c r="F36">
-        <v>0.91100000000000003</v>
-      </c>
-      <c r="J36">
-        <v>2</v>
-      </c>
-      <c r="K36">
-        <v>-1.9883500000000001</v>
-      </c>
-      <c r="L36">
-        <v>0.82299999999999995</v>
-      </c>
-    </row>
-    <row r="37" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D37">
-        <v>3</v>
-      </c>
-      <c r="E37">
-        <v>-2.9767100000000002</v>
-      </c>
-      <c r="F37">
-        <v>0.77700000000000002</v>
-      </c>
-      <c r="J37">
-        <v>3</v>
-      </c>
-      <c r="K37">
-        <v>-2.9810699999999999</v>
-      </c>
-      <c r="L37">
-        <v>0.68600000000000005</v>
-      </c>
-    </row>
-    <row r="38" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D38">
-        <v>2</v>
-      </c>
-      <c r="E38">
-        <v>-1.9855100000000001</v>
-      </c>
-      <c r="F38">
-        <v>0.91100000000000003</v>
-      </c>
-      <c r="J38">
-        <v>2</v>
-      </c>
-      <c r="K38">
-        <v>-1.98956</v>
-      </c>
-      <c r="L38">
-        <v>0.82399999999999995</v>
-      </c>
-    </row>
-    <row r="39" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>-0.98996300000000004</v>
-      </c>
-      <c r="F39">
-        <v>1.044</v>
-      </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
-      <c r="K39">
-        <v>-0.99669799999999997</v>
-      </c>
-      <c r="L39">
-        <v>0.95899999999999996</v>
-      </c>
-    </row>
-    <row r="40" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D40">
+      <c r="E40">
+        <v>-1.40977</v>
+      </c>
+      <c r="F40">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="J40">
+        <v>-1</v>
+      </c>
+      <c r="K40">
+        <v>-1.70855</v>
+      </c>
+      <c r="L40">
+        <v>0.83699999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D41">
         <v>0</v>
       </c>
-      <c r="E40">
-        <v>4.1662000000000001E-3</v>
-      </c>
-      <c r="F40">
-        <v>1.1759999999999999</v>
-      </c>
-      <c r="J40">
+      <c r="E41">
+        <v>-0.41535</v>
+      </c>
+      <c r="F41">
+        <v>1.0189999999999999</v>
+      </c>
+      <c r="J41">
+        <v>-2</v>
+      </c>
+      <c r="K41">
+        <v>-0.71423099999999995</v>
+      </c>
+      <c r="L41">
+        <v>0.96099999999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>-1</v>
+      </c>
+      <c r="E42">
+        <v>0.58041699999999996</v>
+      </c>
+      <c r="F42">
+        <v>1.149</v>
+      </c>
+      <c r="J42">
+        <v>-3</v>
+      </c>
+      <c r="K42">
+        <v>0.27846399999999999</v>
+      </c>
+      <c r="L42">
+        <v>1.099</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>-2</v>
+      </c>
+      <c r="E43">
+        <v>1.57426</v>
+      </c>
+      <c r="F43">
+        <v>1.2829999999999999</v>
+      </c>
+      <c r="J43">
+        <v>-4</v>
+      </c>
+      <c r="K43">
+        <v>1.2700499999999999</v>
+      </c>
+      <c r="L43">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>-3</v>
+      </c>
+      <c r="E44">
+        <v>2.5695399999999999</v>
+      </c>
+      <c r="F44">
+        <v>1.4219999999999999</v>
+      </c>
+      <c r="J44">
+        <v>-5</v>
+      </c>
+      <c r="K44">
+        <v>2.2633700000000001</v>
+      </c>
+      <c r="L44">
+        <v>1.3740000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>-4</v>
+      </c>
+      <c r="E45">
+        <v>3.5644300000000002</v>
+      </c>
+      <c r="F45">
+        <v>1.5529999999999999</v>
+      </c>
+      <c r="J45">
+        <v>-4</v>
+      </c>
+      <c r="K45">
+        <v>1.27153</v>
+      </c>
+      <c r="L45">
+        <v>1.2390000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>-5</v>
+      </c>
+      <c r="E46">
+        <v>4.5615899999999998</v>
+      </c>
+      <c r="F46">
+        <v>1.6879999999999999</v>
+      </c>
+      <c r="J46">
+        <v>-3</v>
+      </c>
+      <c r="K46">
+        <v>0.27963100000000002</v>
+      </c>
+      <c r="L46">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>-4</v>
+      </c>
+      <c r="E47">
+        <v>3.5677400000000001</v>
+      </c>
+      <c r="F47">
+        <v>1.5660000000000001</v>
+      </c>
+      <c r="J47">
+        <v>-2</v>
+      </c>
+      <c r="K47">
+        <v>-0.71310600000000002</v>
+      </c>
+      <c r="L47">
+        <v>0.97499999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>-3</v>
+      </c>
+      <c r="E48">
+        <v>2.5735700000000001</v>
+      </c>
+      <c r="F48">
+        <v>1.4219999999999999</v>
+      </c>
+      <c r="J48">
+        <v>-1</v>
+      </c>
+      <c r="K48">
+        <v>-1.7068700000000001</v>
+      </c>
+      <c r="L48">
+        <v>0.83699999999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>-2</v>
+      </c>
+      <c r="E49">
+        <v>1.57704</v>
+      </c>
+      <c r="F49">
+        <v>1.2869999999999999</v>
+      </c>
+      <c r="J49">
         <v>0</v>
       </c>
-      <c r="K40">
-        <v>-3.1787299999999998E-3</v>
-      </c>
-      <c r="L40">
-        <v>1.095</v>
-      </c>
-    </row>
-    <row r="41" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D41">
+      <c r="K49">
+        <v>-2.7013400000000001</v>
+      </c>
+      <c r="L49">
+        <v>0.69899999999999995</v>
+      </c>
+    </row>
+    <row r="50" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D50">
         <v>-1</v>
       </c>
-      <c r="E41">
-        <v>0.99865300000000001</v>
-      </c>
-      <c r="F41">
-        <v>1.304</v>
-      </c>
-      <c r="J41">
-        <v>-1</v>
-      </c>
-      <c r="K41">
-        <v>0.98945099999999997</v>
-      </c>
-      <c r="L41">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="42" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D42">
-        <v>-2</v>
-      </c>
-      <c r="E42">
-        <v>1.99346</v>
-      </c>
-      <c r="F42">
-        <v>1.4390000000000001</v>
-      </c>
-      <c r="J42">
-        <v>-2</v>
-      </c>
-      <c r="K42">
-        <v>1.98329</v>
-      </c>
-      <c r="L42">
-        <v>1.3580000000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D43">
-        <v>-3</v>
-      </c>
-      <c r="E43">
-        <v>2.9877799999999999</v>
-      </c>
-      <c r="F43">
-        <v>1.5840000000000001</v>
-      </c>
-      <c r="J43">
-        <v>-3</v>
-      </c>
-      <c r="K43">
-        <v>2.9761799999999998</v>
-      </c>
-      <c r="L43">
-        <v>1.494</v>
-      </c>
-    </row>
-    <row r="44" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D44">
-        <v>-4</v>
-      </c>
-      <c r="E44">
-        <v>3.9847700000000001</v>
-      </c>
-      <c r="F44">
-        <v>1.718</v>
-      </c>
-      <c r="J44">
-        <v>-4</v>
-      </c>
-      <c r="K44">
-        <v>3.9709400000000001</v>
-      </c>
-      <c r="L44">
-        <v>1.63</v>
-      </c>
-    </row>
-    <row r="45" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D45">
-        <v>-3</v>
-      </c>
-      <c r="E45">
-        <v>2.9918200000000001</v>
-      </c>
-      <c r="F45">
-        <v>1.573</v>
-      </c>
-      <c r="J45">
-        <v>-3</v>
-      </c>
-      <c r="K45">
-        <v>2.97736</v>
-      </c>
-      <c r="L45">
-        <v>1.494</v>
-      </c>
-    </row>
-    <row r="46" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D46">
-        <v>-2</v>
-      </c>
-      <c r="E46">
-        <v>1.9958499999999999</v>
-      </c>
-      <c r="F46">
-        <v>1.44</v>
-      </c>
-      <c r="J46">
-        <v>-2</v>
-      </c>
-      <c r="K46">
-        <v>1.98481</v>
-      </c>
-      <c r="L46">
-        <v>1.359</v>
-      </c>
-    </row>
-    <row r="47" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D47">
-        <v>-1</v>
-      </c>
-      <c r="E47">
-        <v>1.00142</v>
-      </c>
-      <c r="F47">
-        <v>1.3049999999999999</v>
-      </c>
-      <c r="J47">
-        <v>-1</v>
-      </c>
-      <c r="K47">
-        <v>0.99148199999999997</v>
-      </c>
-      <c r="L47">
-        <v>1.228</v>
-      </c>
-    </row>
-    <row r="48" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D48">
+      <c r="E50">
+        <v>0.58275699999999997</v>
+      </c>
+      <c r="F50">
+        <v>1.153</v>
+      </c>
+    </row>
+    <row r="51" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D51">
         <v>0</v>
       </c>
-      <c r="E48">
-        <v>5.9465799999999999E-3</v>
-      </c>
-      <c r="F48">
-        <v>1.17</v>
-      </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="K48">
-        <v>-1.9954500000000002E-3</v>
-      </c>
-      <c r="L48">
-        <v>1.093</v>
-      </c>
-    </row>
-    <row r="50" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="E50">
-        <f>SLOPE(F34:F48,D34:D48)</f>
-        <v>-0.13356361607142858</v>
-      </c>
-      <c r="F50">
-        <f>SLOPE(F34:F48,E34:E48)</f>
-        <v>0.13428172907023248</v>
-      </c>
-      <c r="K50">
-        <f>SLOPE(L34:L48,J34:J48)</f>
-        <v>-0.13428013392857141</v>
-      </c>
-      <c r="L50">
-        <f>SLOPE(L34:L48,K34:K48)</f>
-        <v>0.13520264780016397</v>
-      </c>
-    </row>
-    <row r="51" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="E51" t="s">
+      <c r="E51">
+        <v>-0.41276499999999999</v>
+      </c>
+      <c r="F51">
+        <v>1.0209999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53">
+        <f>SLOPE(F37:F51,D37:D51)</f>
+        <v>-0.13434415584415585</v>
+      </c>
+      <c r="F53">
+        <f>SLOPE(F37:F51,E37:E51)</f>
+        <v>0.13501478873891026</v>
+      </c>
+      <c r="I53" t="s">
+        <v>56</v>
+      </c>
+      <c r="K53">
+        <f>SLOPE(L37:L51,J37:J51)</f>
+        <v>-0.13429232283464571</v>
+      </c>
+      <c r="L53">
+        <f>SLOPE(L37:L51,K37:K51)</f>
+        <v>0.13519771607008962</v>
+      </c>
+    </row>
+    <row r="54" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
         <v>32</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F54" t="s">
         <v>33</v>
       </c>
-      <c r="K51" t="s">
+      <c r="K54" t="s">
         <v>32</v>
       </c>
-      <c r="L51" t="s">
+      <c r="L54" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="55" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
+        <v>53</v>
+      </c>
+      <c r="E55">
+        <f>RSQ(E35:E51,D35:D51)</f>
+        <v>0.9999995026675762</v>
+      </c>
+      <c r="F55">
+        <f>RSQ(F35:F51,D35:D51)</f>
+        <v>0.99985031882025088</v>
+      </c>
+      <c r="I55" t="s">
+        <v>53</v>
+      </c>
+      <c r="K55">
+        <f>RSQ(K35:K51,J35:J51)</f>
+        <v>0.99999941585054453</v>
+      </c>
+      <c r="L55">
+        <f>RSQ(L35:L51,J35:J51)</f>
+        <v>0.99968262071779779</v>
+      </c>
+    </row>
+    <row r="56" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56">
+        <v>-0.13356361607142858</v>
+      </c>
+      <c r="F56">
+        <v>0.13428172907023248</v>
+      </c>
+      <c r="I56" t="s">
+        <v>52</v>
+      </c>
+      <c r="K56">
+        <v>-0.13428013392857141</v>
+      </c>
+      <c r="L56">
+        <v>0.13520264780016397</v>
+      </c>
+    </row>
+    <row r="57" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>54</v>
+      </c>
+      <c r="E57">
+        <f>E53-E56</f>
+        <v>-7.8053977272726782E-4</v>
+      </c>
+      <c r="F57">
+        <f>F53-F56</f>
+        <v>7.3305966867778793E-4</v>
+      </c>
+      <c r="I57" t="s">
+        <v>54</v>
+      </c>
+      <c r="K57">
+        <f>K53-K56</f>
+        <v>-1.2188906074295236E-5</v>
+      </c>
+      <c r="L57">
+        <f>L53-L56</f>
+        <v>-4.9317300743478842E-6</v>
+      </c>
+    </row>
+    <row r="58" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>55</v>
+      </c>
+      <c r="E58" s="8">
+        <f>(E56-E53)/((E53+E56)/2)</f>
+        <v>-5.8269289251766049E-3</v>
+      </c>
+      <c r="F58" s="8">
+        <f>(F56-F53)/((F53+F56)/2)</f>
+        <v>-5.4442565736949177E-3</v>
+      </c>
+      <c r="I58" t="s">
+        <v>55</v>
+      </c>
+      <c r="K58" s="8">
+        <f>(K56-K53)/((K53+K56)/2)</f>
+        <v>-9.0768101995219883E-5</v>
+      </c>
+      <c r="L58" s="8">
+        <f>(L56-L53)/((L53+L56)/2)</f>
+        <v>3.6477244362838805E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
         <v>35</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D60" t="s">
         <v>31</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E60" t="s">
         <v>29</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F60" t="s">
         <v>30</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I60" t="s">
         <v>36</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J60" t="s">
         <v>31</v>
       </c>
-      <c r="K55" t="s">
+      <c r="K60" t="s">
         <v>29</v>
       </c>
-      <c r="L55" t="s">
+      <c r="L60" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>8.7660500000000002E-2</v>
-      </c>
-      <c r="F58">
-        <v>1.1419999999999999</v>
-      </c>
-      <c r="J58">
-        <v>0</v>
-      </c>
-      <c r="K58">
-        <v>-4.37863E-2</v>
-      </c>
-      <c r="L58">
-        <v>1.121</v>
-      </c>
-    </row>
-    <row r="59" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59">
-        <v>-0.90350299999999995</v>
-      </c>
-      <c r="F59">
-        <v>1.0009999999999999</v>
-      </c>
-      <c r="J59">
-        <v>0.5</v>
-      </c>
-      <c r="K59">
-        <v>-0.54621900000000001</v>
-      </c>
-      <c r="L59">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="60" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D60">
-        <v>2</v>
-      </c>
-      <c r="E60">
-        <v>-1.8989400000000001</v>
-      </c>
-      <c r="F60">
-        <v>0.874</v>
-      </c>
-      <c r="J60">
-        <v>1</v>
-      </c>
-      <c r="K60">
-        <v>-1.0459400000000001</v>
-      </c>
-      <c r="L60">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="61" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D61">
-        <v>3</v>
-      </c>
-      <c r="E61">
-        <v>-2.8938000000000001</v>
-      </c>
-      <c r="F61">
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="J61">
-        <v>0.5</v>
-      </c>
-      <c r="K61">
-        <v>-0.54433200000000004</v>
-      </c>
-      <c r="L61">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="62" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="D62">
-        <v>2</v>
-      </c>
-      <c r="E62">
-        <v>-1.9026000000000001</v>
-      </c>
-      <c r="F62">
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="J62">
-        <v>0</v>
-      </c>
-      <c r="K62">
-        <v>-4.49641E-2</v>
-      </c>
-      <c r="L62">
-        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="63" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>-0.90710100000000005</v>
+        <v>-2.7769900000000001</v>
       </c>
       <c r="F63">
-        <v>1.008</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="J63">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="K63">
-        <v>0.45691900000000002</v>
+        <v>-0.71184099999999995</v>
       </c>
       <c r="L63">
-        <v>1.333</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="64" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>-3.7716699999999999</v>
+      </c>
+      <c r="F64">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="J64">
+        <v>0.5</v>
+      </c>
+      <c r="K64">
+        <v>-1.20709</v>
+      </c>
+      <c r="L64">
+        <v>0.73099999999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <v>-4.7677399999999999</v>
+      </c>
+      <c r="F65">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="K65">
+        <v>-1.7056199999999999</v>
+      </c>
+      <c r="L65">
+        <v>0.50900000000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>-3.7719200000000002</v>
+      </c>
+      <c r="F66">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="J66">
+        <v>0.5</v>
+      </c>
+      <c r="K66">
+        <v>-1.20983</v>
+      </c>
+      <c r="L66">
+        <v>0.73099999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D67">
         <v>0</v>
       </c>
-      <c r="E64">
-        <v>8.8358800000000001E-2</v>
-      </c>
-      <c r="F64">
-        <v>1.1359999999999999</v>
-      </c>
-      <c r="J64">
+      <c r="E67">
+        <v>-2.7754599999999998</v>
+      </c>
+      <c r="F67">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>-0.71074300000000001</v>
+      </c>
+      <c r="L67">
+        <v>0.93899999999999995</v>
+      </c>
+    </row>
+    <row r="68" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D68">
         <v>-1</v>
       </c>
-      <c r="K64">
-        <v>0.95511500000000005</v>
-      </c>
-      <c r="L64">
-        <v>1.542</v>
-      </c>
-    </row>
-    <row r="65" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D65">
+      <c r="E68">
+        <v>-1.7803199999999999</v>
+      </c>
+      <c r="F68">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="J68">
+        <v>-0.5</v>
+      </c>
+      <c r="K68">
+        <v>-0.21573000000000001</v>
+      </c>
+      <c r="L68">
+        <v>1.1459999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>-2</v>
+      </c>
+      <c r="E69">
+        <v>-0.78536099999999998</v>
+      </c>
+      <c r="F69">
+        <v>1.02</v>
+      </c>
+      <c r="J69">
         <v>-1</v>
       </c>
-      <c r="E65">
-        <v>1.08449</v>
-      </c>
-      <c r="F65">
-        <v>1.266</v>
-      </c>
-      <c r="J65">
+      <c r="K69">
+        <v>0.28158100000000003</v>
+      </c>
+      <c r="L69">
+        <v>1.3520000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>-3</v>
+      </c>
+      <c r="E70">
+        <v>0.20873700000000001</v>
+      </c>
+      <c r="F70">
+        <v>1.149</v>
+      </c>
+      <c r="J70">
         <v>-1.5</v>
       </c>
-      <c r="K65">
-        <v>1.4554499999999999</v>
-      </c>
-      <c r="L65">
-        <v>1.7569999999999999</v>
-      </c>
-    </row>
-    <row r="66" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D66">
+      <c r="K70">
+        <v>0.78152500000000003</v>
+      </c>
+      <c r="L70">
+        <v>1.524</v>
+      </c>
+    </row>
+    <row r="71" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>-4</v>
+      </c>
+      <c r="E71">
+        <v>1.2029700000000001</v>
+      </c>
+      <c r="F71">
+        <v>1.258</v>
+      </c>
+      <c r="J71">
+        <v>-1</v>
+      </c>
+      <c r="K71">
+        <v>0.281246</v>
+      </c>
+      <c r="L71">
+        <v>1.335</v>
+      </c>
+    </row>
+    <row r="72" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>-3</v>
+      </c>
+      <c r="E72">
+        <v>0.211674</v>
+      </c>
+      <c r="F72">
+        <v>1.1479999999999999</v>
+      </c>
+      <c r="J72">
+        <v>-0.5</v>
+      </c>
+      <c r="K72">
+        <v>-0.21412500000000001</v>
+      </c>
+      <c r="L72">
+        <v>1.129</v>
+      </c>
+    </row>
+    <row r="73" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D73">
         <v>-2</v>
       </c>
-      <c r="E66">
-        <v>2.0805699999999998</v>
-      </c>
-      <c r="F66">
-        <v>1.405</v>
-      </c>
-      <c r="J66">
+      <c r="E73">
+        <v>-0.78347900000000004</v>
+      </c>
+      <c r="F73">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>-0.71005600000000002</v>
+      </c>
+      <c r="L73">
+        <v>0.93200000000000005</v>
+      </c>
+    </row>
+    <row r="74" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D74">
         <v>-1</v>
       </c>
-      <c r="K66">
-        <v>0.956229</v>
-      </c>
-      <c r="L66">
-        <v>1.542</v>
-      </c>
-    </row>
-    <row r="67" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D67">
-        <v>-3</v>
-      </c>
-      <c r="E67">
-        <v>3.07639</v>
-      </c>
-      <c r="F67">
-        <v>1.5349999999999999</v>
-      </c>
-      <c r="J67">
-        <v>-0.5</v>
-      </c>
-      <c r="K67">
-        <v>0.456013</v>
-      </c>
-      <c r="L67">
-        <v>1.327</v>
-      </c>
-    </row>
-    <row r="68" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D68">
-        <v>-2</v>
-      </c>
-      <c r="E68">
-        <v>2.08467</v>
-      </c>
-      <c r="F68">
-        <v>1.4039999999999999</v>
-      </c>
-      <c r="J68">
+      <c r="E74">
+        <v>-1.7779700000000001</v>
+      </c>
+      <c r="F74">
+        <v>0.89200000000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D75">
         <v>0</v>
       </c>
-      <c r="K68">
-        <v>-4.39675E-2</v>
-      </c>
-      <c r="L68">
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="69" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D69">
-        <v>-1</v>
-      </c>
-      <c r="E69">
-        <v>1.08897</v>
-      </c>
-      <c r="F69">
-        <v>1.2669999999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>9.2154E-2</v>
-      </c>
-      <c r="F70">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="74" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="E74">
-        <f>SLOPE(F58:F70,D58:D70)</f>
+      <c r="E75">
+        <v>-2.7726700000000002</v>
+      </c>
+      <c r="F75">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>56</v>
+      </c>
+      <c r="E79">
+        <f>SLOPE(F63:F75,D63:D75)</f>
+        <v>-0.12548418972332015</v>
+      </c>
+      <c r="F79">
+        <f>SLOPE(F63:F75,E63:E75)</f>
+        <v>0.12608102115425956</v>
+      </c>
+      <c r="I79" t="s">
+        <v>56</v>
+      </c>
+      <c r="K79">
+        <f>SLOPE(L63:L73,J63:J73)</f>
+        <v>-0.40648800000000013</v>
+      </c>
+      <c r="L79">
+        <f>SLOPE(L63:L73,K63:K73)</f>
+        <v>0.40890683932975469</v>
+      </c>
+    </row>
+    <row r="80" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>32</v>
+      </c>
+      <c r="F80" t="s">
+        <v>33</v>
+      </c>
+      <c r="K80" t="s">
+        <v>32</v>
+      </c>
+      <c r="L80" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="81" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>53</v>
+      </c>
+      <c r="E81">
+        <f>RSQ(E61:E77,D61:D77)</f>
+        <v>0.99999912922733192</v>
+      </c>
+      <c r="F81">
+        <f>RSQ(F61:F77,D61:D77)</f>
+        <v>0.99926865114626817</v>
+      </c>
+      <c r="I81" t="s">
+        <v>53</v>
+      </c>
+      <c r="K81">
+        <f>RSQ(K61:K77,J61:J77)</f>
+        <v>0.99999739299042334</v>
+      </c>
+      <c r="L81">
+        <f>RSQ(L61:L77,J61:J77)</f>
+        <v>0.99887266950558373</v>
+      </c>
+    </row>
+    <row r="82" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>52</v>
+      </c>
+      <c r="E82">
         <v>-0.13221052631578945</v>
       </c>
-      <c r="F74">
-        <f>SLOPE(F58:F70,E58:E70)</f>
+      <c r="F82">
         <v>0.13280936201772017</v>
       </c>
-      <c r="K74">
-        <f>SLOPE(L58:L68,J58:J68)</f>
+      <c r="I82" t="s">
+        <v>52</v>
+      </c>
+      <c r="K82">
         <v>-0.41143199999999991</v>
       </c>
-      <c r="L74">
-        <f>SLOPE(L58:L68,K58:K68)</f>
+      <c r="L82">
         <v>0.41117825380426376</v>
       </c>
     </row>
-    <row r="75" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="E75" t="s">
-        <v>32</v>
-      </c>
-      <c r="F75" t="s">
-        <v>33</v>
-      </c>
-      <c r="K75" t="s">
-        <v>32</v>
-      </c>
-      <c r="L75" t="s">
-        <v>33</v>
+    <row r="83" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>54</v>
+      </c>
+      <c r="E83">
+        <f>E79-E82</f>
+        <v>6.7263365924692953E-3</v>
+      </c>
+      <c r="F83">
+        <f>F79-F82</f>
+        <v>-6.7283408634606079E-3</v>
+      </c>
+      <c r="I83" t="s">
+        <v>54</v>
+      </c>
+      <c r="K83">
+        <f>K79-K82</f>
+        <v>4.9439999999997819E-3</v>
+      </c>
+      <c r="L83">
+        <f>L79-L82</f>
+        <v>-2.2714144745090703E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>55</v>
+      </c>
+      <c r="E84" s="8">
+        <f>(E82-E79)/((E79+E82)/2)</f>
+        <v>5.2203915515663564E-2</v>
+      </c>
+      <c r="F84" s="8">
+        <f>(F82-F79)/((F79+F82)/2)</f>
+        <v>5.1978298931181235E-2</v>
+      </c>
+      <c r="I84" t="s">
+        <v>55</v>
+      </c>
+      <c r="K84" s="8">
+        <f>(K82-K79)/((K79+K82)/2)</f>
+        <v>1.2089201877933739E-2</v>
+      </c>
+      <c r="L84" s="8">
+        <f>(L82-L79)/((L79+L82)/2)</f>
+        <v>5.5394604621544444E-3</v>
       </c>
     </row>
   </sheetData>
@@ -3098,7 +3401,7 @@
   <dimension ref="C4:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3120,78 +3423,78 @@
       <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="15">
         <f>calibration!E27</f>
-        <v>-0.27211363636363639</v>
-      </c>
-      <c r="E5" s="6">
+        <v>-0.26889473684210524</v>
+      </c>
+      <c r="E5" s="15">
         <f>calibration!F27</f>
-        <v>0.27375622714345149</v>
+        <v>0.26773623149939174</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="15">
         <f>calibration!K27</f>
-        <v>-0.27455681818181821</v>
-      </c>
-      <c r="E6" s="6">
+        <v>-0.26820424107142854</v>
+      </c>
+      <c r="E6" s="15">
         <f>calibration!L27</f>
-        <v>0.27318441842715224</v>
+        <v>0.26755083133801272</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="6">
-        <f>calibration!E50</f>
-        <v>-0.13356361607142858</v>
-      </c>
-      <c r="E7" s="6">
-        <f>calibration!F50</f>
-        <v>0.13428172907023248</v>
+      <c r="D7" s="15">
+        <f>calibration!E53</f>
+        <v>-0.13434415584415585</v>
+      </c>
+      <c r="E7" s="15">
+        <f>calibration!F53</f>
+        <v>0.13501478873891026</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="6">
-        <f>calibration!K50</f>
-        <v>-0.13428013392857141</v>
-      </c>
-      <c r="E8" s="6">
-        <f>calibration!L50</f>
-        <v>0.13520264780016397</v>
+      <c r="D8" s="15">
+        <f>calibration!K53</f>
+        <v>-0.13429232283464571</v>
+      </c>
+      <c r="E8" s="15">
+        <f>calibration!L53</f>
+        <v>0.13519771607008962</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="6">
-        <f>calibration!E74</f>
-        <v>-0.13221052631578945</v>
-      </c>
-      <c r="E9" s="6">
-        <f>calibration!F74</f>
-        <v>0.13280936201772017</v>
+      <c r="D9" s="15">
+        <f>calibration!E79</f>
+        <v>-0.12548418972332015</v>
+      </c>
+      <c r="E9" s="15">
+        <f>calibration!F79</f>
+        <v>0.12608102115425956</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="6">
-        <f>calibration!K74</f>
-        <v>-0.41143199999999991</v>
-      </c>
-      <c r="E10" s="6">
-        <f>calibration!L74</f>
-        <v>0.41117825380426376</v>
+      <c r="D10" s="15">
+        <f>calibration!K79</f>
+        <v>-0.40648800000000013</v>
+      </c>
+      <c r="E10" s="15">
+        <f>calibration!L79</f>
+        <v>0.40890683932975469</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
@@ -3230,90 +3533,90 @@
       <c r="C16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="6">
-        <v>-1.46188E-2</v>
-      </c>
-      <c r="E16" s="6">
+      <c r="D16" s="15">
+        <v>-2.2238899999999999E-2</v>
+      </c>
+      <c r="E16" s="14">
         <f>SWController!$D$17</f>
-        <v>12.989869513449323</v>
+        <v>14.900643377012043</v>
       </c>
       <c r="F16" s="7">
-        <v>-1.3367500000000001</v>
+        <v>-1.50674</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="6">
-        <v>7.0011900000000002E-2</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="D17" s="15">
+        <v>-3.2907600000000002E-2</v>
+      </c>
+      <c r="E17" s="14">
         <f>SWController!$E$17</f>
-        <v>10.714680503359387</v>
+        <v>15.925377380995291</v>
       </c>
       <c r="F17" s="7">
-        <v>-1.12473</v>
+        <v>-1.58768</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="6">
-        <v>6.8504800000000005E-2</v>
-      </c>
-      <c r="E18" s="6">
+      <c r="D18" s="15">
+        <v>4.5411200000000001E-4</v>
+      </c>
+      <c r="E18" s="14">
         <f>SWController!$F$17</f>
-        <v>4.1816546761306883</v>
+        <v>11.610850871062473</v>
       </c>
       <c r="F18" s="7">
-        <v>-0.44009199999999998</v>
+        <v>-1.1766700000000001</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="6">
-        <v>2.24368E-2</v>
-      </c>
-      <c r="E19" s="6">
+      <c r="D19" s="15">
+        <v>1.21177E-2</v>
+      </c>
+      <c r="E19" s="14">
         <f>SWController!$G$17</f>
-        <v>26.346065207231756</v>
+        <v>29.539583568552928</v>
       </c>
       <c r="F19" s="7">
-        <v>-2.7015899999999999</v>
+        <v>-3.0303200000000001</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="6">
-        <v>-0.21193300000000001</v>
-      </c>
-      <c r="E20" s="6">
+      <c r="D20" s="15">
+        <v>0.123263</v>
+      </c>
+      <c r="E20" s="14">
         <f>SWController!$H$17</f>
-        <v>26.622797180376637</v>
+        <v>27.595350728731248</v>
       </c>
       <c r="F20" s="7">
-        <v>-2.6579799999999998</v>
+        <v>-2.8785599999999998</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="8">
-        <v>0.140767</v>
-      </c>
-      <c r="E21" s="6">
+      <c r="D21" s="15">
+        <v>3.2462900000000003E-2</v>
+      </c>
+      <c r="E21" s="14">
         <f>SWController!$I$17</f>
-        <v>7.1724008241095758</v>
+        <v>11.840841021545243</v>
       </c>
       <c r="F21" s="7">
-        <v>-0.78510800000000003</v>
+        <v>-1.18906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>